<commit_message>
added caching of KS deaths
</commit_message>
<xml_diff>
--- a/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
+++ b/snapshot/fdcf2531-4c3e-5c02-b63c-ee160ead6dea.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\AKTUALNI PODATKI - KORONA\Za objavo na GOV.SI\ang\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654FC9E3-1792-4C0A-8F62-962376F54392}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 podatki" sheetId="1" r:id="rId1"/>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/\ m/\ yyyy;@"/>
   </numFmts>
@@ -132,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -198,6 +199,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -389,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:J71" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:J73" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J73" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -403,16 +413,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" name="Tested (all)" dataDxfId="8"/>
-    <tableColumn id="3" name="Tested (daily)" dataDxfId="7"/>
-    <tableColumn id="4" name="Positive (all)" dataDxfId="6"/>
-    <tableColumn id="5" name="Positive (daily)" dataDxfId="5"/>
-    <tableColumn id="6" name="All hospitalized on certain day" dataDxfId="4"/>
-    <tableColumn id="7" name="All persons in intensive care on certain day" dataDxfId="3"/>
-    <tableColumn id="10" name="Discharged" dataDxfId="2"/>
-    <tableColumn id="8" name="Deaths (all)" dataDxfId="1"/>
-    <tableColumn id="9" name="Deaths (daily)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tested (all)" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tested (daily)" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Positive (all)" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Positive (daily)" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="All hospitalized on certain day" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="All persons in intensive care on certain day" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Discharged" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deaths (all)" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Deaths (daily)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -685,11 +695,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71:J71"/>
+      <selection activeCell="J73" sqref="A73:J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2979,6 +2989,70 @@
         <v>1</v>
       </c>
     </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="23">
+        <v>43972</v>
+      </c>
+      <c r="B72" s="24">
+        <v>73742</v>
+      </c>
+      <c r="C72" s="25">
+        <v>882</v>
+      </c>
+      <c r="D72" s="25">
+        <v>1468</v>
+      </c>
+      <c r="E72" s="25">
+        <v>0</v>
+      </c>
+      <c r="F72" s="25">
+        <v>21</v>
+      </c>
+      <c r="G72" s="25">
+        <v>4</v>
+      </c>
+      <c r="H72" s="25">
+        <v>0</v>
+      </c>
+      <c r="I72" s="25">
+        <v>106</v>
+      </c>
+      <c r="J72" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="20">
+        <v>43973</v>
+      </c>
+      <c r="B73" s="21">
+        <v>74419</v>
+      </c>
+      <c r="C73" s="22">
+        <v>677</v>
+      </c>
+      <c r="D73" s="22">
+        <v>1468</v>
+      </c>
+      <c r="E73" s="22">
+        <v>0</v>
+      </c>
+      <c r="F73" s="22">
+        <v>19</v>
+      </c>
+      <c r="G73" s="22">
+        <v>4</v>
+      </c>
+      <c r="H73" s="22">
+        <v>2</v>
+      </c>
+      <c r="I73" s="22">
+        <v>106</v>
+      </c>
+      <c r="J73" s="22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>